<commit_message>
actualizado ficheiro da proposta inicial
</commit_message>
<xml_diff>
--- a/Documentacao/Estimativas.xlsx
+++ b/Documentacao/Estimativas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\ISEL\PS\ProjectoFInal\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A179DFC7-EF46-40EF-9CD5-C52892412D8E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7139D3C1-CF47-4426-A37E-E816855111CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{7164626F-C57A-4903-BF5E-34B0018640FB}"/>
   </bookViews>
@@ -220,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -402,11 +402,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -425,9 +458,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -449,13 +479,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968F1FF1-E007-4E70-811E-024FA45B8541}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D29"/>
     </sheetView>
   </sheetViews>
@@ -790,13 +836,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
@@ -804,13 +850,13 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>43899</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
@@ -887,15 +933,15 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+    <row r="11" spans="2:6" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21">
         <f t="shared" si="0"/>
         <v>43955</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -937,7 +983,7 @@
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -949,9 +995,7 @@
       <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
@@ -968,7 +1012,7 @@
         <f t="shared" si="0"/>
         <v>44004</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="6"/>
@@ -981,7 +1025,7 @@
         <f t="shared" si="0"/>
         <v>44011</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="6"/>
       <c r="F19" s="2"/>
     </row>
@@ -990,7 +1034,7 @@
         <f t="shared" si="0"/>
         <v>44018</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="6"/>
       <c r="F20" s="2"/>
     </row>
@@ -999,7 +1043,7 @@
         <f t="shared" si="0"/>
         <v>44025</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="6"/>
       <c r="F21" s="2"/>
     </row>
@@ -1008,7 +1052,7 @@
         <f t="shared" si="0"/>
         <v>44032</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="6"/>
       <c r="F22" s="2"/>
     </row>
@@ -1020,7 +1064,9 @@
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
@@ -1073,14 +1119,14 @@
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="9">
+      <c r="B29" s="8">
         <f>+B28+7</f>
         <v>44081</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1088,7 +1134,10 @@
       <c r="E30" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C18:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>